<commit_message>
add new laba bim bom
</commit_message>
<xml_diff>
--- a/1.2.5/rotor_inertia.xlsx
+++ b/1.2.5/rotor_inertia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\labs\1.2.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CF4A47-46EC-4288-AF68-7A91D68C2A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D90488-55C7-4848-9356-1C88D1BC13B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29250" yWindow="2970" windowWidth="8385" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -405,8 +405,8 @@
         <v>4.01</v>
       </c>
       <c r="E2">
-        <f>A2*B2^2/32*C2*C2/D2/D2</f>
-        <v>1.9390936915782164E-4</v>
+        <f>A2*B2^2/8*C2*C2/D2/D2</f>
+        <v>7.7563747663128655E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>